<commit_message>
[UPDATE] Success to save excel file, and load excel file.
</commit_message>
<xml_diff>
--- a/RPG_Game/GameData.xlsx
+++ b/RPG_Game/GameData.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re432579294f74367"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" r:id="R173f01bc99dc4936"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,9 +10,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetData>
-    <x:c r="B2" t="str">
-      <x:v>Hello, Excel!</x:v>
-    </x:c>
+    <x:row>
+      <x:c t="str">
+        <x:v>Hello</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>World</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>엑셀저장 테스트</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
 </x:worksheet>
 </file>
</xml_diff>